<commit_message>
Added schedule for Adam Furbee
</commit_message>
<xml_diff>
--- a/Availability.xlsx
+++ b/Availability.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27106"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Storage/SoftwareEngineering/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="27520" windowHeight="11500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Day of the Week</t>
   </si>
@@ -85,6 +98,12 @@
   </si>
   <si>
     <t>MN = Midnight</t>
+  </si>
+  <si>
+    <t>5pm-MN</t>
+  </si>
+  <si>
+    <t>8am-MN</t>
   </si>
 </sst>
 </file>
@@ -137,13 +156,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,12 +220,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -236,12 +255,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -448,19 +467,19 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -473,36 +492,36 @@
       <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -528,37 +547,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -580,7 +620,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -592,7 +632,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Whoops, filled out my info in josh's field. Correcting.
</commit_message>
<xml_diff>
--- a/Availability.xlsx
+++ b/Availability.xlsx
@@ -467,7 +467,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -551,27 +551,6 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -601,6 +580,27 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a phone numbers field
</commit_message>
<xml_diff>
--- a/Availability.xlsx
+++ b/Availability.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thamer\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iakav\Documents\GitHub\SoftwareEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Day of the Week</t>
   </si>
@@ -167,6 +167,33 @@
   </si>
   <si>
     <t>t_alhusain@yahoo.com</t>
+  </si>
+  <si>
+    <t>Patrick Starkey</t>
+  </si>
+  <si>
+    <t>9 am-MN</t>
+  </si>
+  <si>
+    <t>9-MN</t>
+  </si>
+  <si>
+    <t>iakavas@live.com</t>
+  </si>
+  <si>
+    <t>10am-3</t>
+  </si>
+  <si>
+    <t>9am-12</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>281-797-7242</t>
+  </si>
+  <si>
+    <t>9am-1230 &amp; 2-9</t>
   </si>
 </sst>
 </file>
@@ -542,20 +569,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -596,6 +625,9 @@
       <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>43</v>
       </c>
@@ -795,6 +827,38 @@
       </c>
       <c r="J10" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -806,9 +870,10 @@
   <hyperlinks>
     <hyperlink ref="J10" r:id="rId1"/>
     <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>